<commit_message>
add new function:final monster
</commit_message>
<xml_diff>
--- a/物品合成.xlsx
+++ b/物品合成.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LAB1223\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12285"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="11020"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
@@ -237,7 +232,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -579,7 +574,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -593,17 +588,17 @@
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="45.125" customWidth="1"/>
-    <col min="4" max="4" width="24.875" customWidth="1"/>
-    <col min="5" max="5" width="27.5" customWidth="1"/>
-    <col min="6" max="6" width="25.375" customWidth="1"/>
-    <col min="7" max="7" width="24.5" customWidth="1"/>
+    <col min="3" max="3" width="45.08984375" customWidth="1"/>
+    <col min="4" max="4" width="24.90625" customWidth="1"/>
+    <col min="5" max="5" width="27.453125" customWidth="1"/>
+    <col min="6" max="6" width="25.36328125" customWidth="1"/>
+    <col min="7" max="7" width="24.453125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -626,7 +621,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>21</v>
@@ -647,7 +642,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -667,7 +662,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>31</v>
@@ -685,7 +680,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -702,7 +697,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>45</v>
@@ -717,7 +712,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -734,7 +729,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
         <v>49</v>
@@ -749,7 +744,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -766,14 +761,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -786,7 +781,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
       <c r="A12" s="1"/>
       <c r="B12" s="3" t="s">
         <v>27</v>

</xml_diff>

<commit_message>
synthesisbar connect with backpack
</commit_message>
<xml_diff>
--- a/物品合成.xlsx
+++ b/物品合成.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4506"/>
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19420" windowHeight="11020"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="19416" windowHeight="11016"/>
   </bookViews>
   <sheets>
     <sheet name="工作表1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="54">
   <si>
     <t>工具列</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -226,14 +226,22 @@
   </si>
   <si>
     <t>新手教學手冊*1,火法杖*1,冰法杖*1,露水*1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>黃金十字鎬</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t xml:space="preserve"> 樹枝*2,燧石*2,黃金*1</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="4">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -362,7 +370,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -397,7 +405,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -574,31 +582,32 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G12"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="I1" sqref="I1:I1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="16.2"/>
   <cols>
     <col min="2" max="2" width="31" customWidth="1"/>
-    <col min="3" max="3" width="45.08984375" customWidth="1"/>
-    <col min="4" max="4" width="24.90625" customWidth="1"/>
-    <col min="5" max="5" width="27.453125" customWidth="1"/>
-    <col min="6" max="6" width="25.36328125" customWidth="1"/>
-    <col min="7" max="7" width="24.453125" customWidth="1"/>
+    <col min="3" max="3" width="45.109375" customWidth="1"/>
+    <col min="4" max="4" width="24.88671875" customWidth="1"/>
+    <col min="5" max="5" width="27.44140625" customWidth="1"/>
+    <col min="6" max="6" width="25.33203125" customWidth="1"/>
+    <col min="7" max="7" width="24.44140625" customWidth="1"/>
+    <col min="8" max="8" width="27.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:8">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -620,8 +629,11 @@
       <c r="G1" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H1" s="2" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
       <c r="A2" s="1"/>
       <c r="B2" s="1" t="s">
         <v>21</v>
@@ -641,8 +653,11 @@
       <c r="G2" s="1" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.4">
+      <c r="H2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
       <c r="A3" s="2" t="s">
         <v>8</v>
       </c>
@@ -662,7 +677,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:8">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
         <v>31</v>
@@ -680,7 +695,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:8">
       <c r="A5" s="2" t="s">
         <v>9</v>
       </c>
@@ -697,7 +712,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:8">
       <c r="A6" s="1"/>
       <c r="B6" s="3" t="s">
         <v>45</v>
@@ -712,7 +727,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:8">
       <c r="A7" s="2" t="s">
         <v>16</v>
       </c>
@@ -729,7 +744,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:8">
       <c r="A8" s="1"/>
       <c r="B8" s="3" t="s">
         <v>49</v>
@@ -744,7 +759,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:8">
       <c r="A9" s="2" t="s">
         <v>3</v>
       </c>
@@ -761,14 +776,14 @@
         <v>7</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="16.5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="A10" s="1"/>
       <c r="B10" s="2"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:8">
       <c r="A11" s="2" t="s">
         <v>25</v>
       </c>
@@ -781,7 +796,7 @@
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:8">
       <c r="A12" s="1"/>
       <c r="B12" s="3" t="s">
         <v>27</v>

</xml_diff>